<commit_message>
Included the las course
This survey includes the last course
</commit_message>
<xml_diff>
--- a/responses/Simulador_SO_Responses.xlsx
+++ b/responses/Simulador_SO_Responses.xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clopezp\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="9615" windowHeight="6690"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Form Responses 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="155">
   <si>
     <t>Timestamp</t>
   </si>
@@ -419,22 +427,80 @@
   </si>
   <si>
     <t>La curva de aprendizaje fue todo un desafío. Sinceramente, fue muy agotador y agobiante, obviamente todo el curso fue un constante reto. Por lo general, es de esa forma cuando más aprende uno. Sin embargo, era tal la velocidad del curso y las clases que no dejaba mucho espacio para preguntas y respuestas con el profesor, tampoco para resolver dudas. El tiempo era tal que sólo estaban la lección y un ejercicio/reto por clase, en el cual solo recibía cierto número de alumnos. Entiendo el objetivo. Presionarnos a dar más. Pero para a quien de verdad se le dificulte o se sienta estancado, es ahí donde se vuelve un verdadero martirio al no poder entregar ni un solo reto, afectando sus oportunidades de sacar una buena calificación en clase. Sólo eso. Dejando esos aspectos de lado, el profesor es muy bueno, sabe bastante.</t>
+  </si>
+  <si>
+    <t>Que sería complejo</t>
+  </si>
+  <si>
+    <t>Incertidumbre</t>
+  </si>
+  <si>
+    <t>No sabía si estaba preparado</t>
+  </si>
+  <si>
+    <t>No sabía exactamente la magnitud</t>
+  </si>
+  <si>
+    <t>No estaba alineado a la materia</t>
+  </si>
+  <si>
+    <t>Reto</t>
+  </si>
+  <si>
+    <t>Me gustó saber desde el principio que iba a realizar</t>
+  </si>
+  <si>
+    <t>Espectativa</t>
+  </si>
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Ppresentar ejemplos reales o similares a la vida de un programador.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Super  buen aprendizaje! </t>
+  </si>
+  <si>
+    <t>excelente manera de dar clases, gracias</t>
+  </si>
+  <si>
+    <t>Excelente profesor Pimentel, gracias por aportar de sus conocimientos y dejarlo en nosotros, a mi parecer y por mis gustos con el diseño web le puedo decir que fue una de mis materias favoritas</t>
+  </si>
+  <si>
+    <t>Para futuras generaciones creo que es indispensable conocer todo lo relacionado con Web, y enseñar otras cosas</t>
+  </si>
+  <si>
+    <t>Excelente estrategia, al hacer parte Web se pueden hacer cosas sorprendentes</t>
+  </si>
+  <si>
+    <t>Me gusto mucho por que hacíamos practicas para luego agregarlo al sistema.</t>
+  </si>
+  <si>
+    <t>aprender un framework de back-end o front-end nos ayudaría a aumentar nuestros conocimientos mucho mas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En lo personal creo que es una buena estrategia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aprendes a ser autodidacta </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -444,40 +510,45 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -667,26 +738,29 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:K72"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H74" sqref="H74:H76"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col customWidth="1" min="1" max="17" width="21.57"/>
+    <col min="1" max="17" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -721,9 +795,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>43750.55791256945</v>
+        <v>43750.557912569449</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>11</v>
@@ -747,7 +821,7 @@
         <v>13</v>
       </c>
       <c r="I2" s="3">
-        <v>2013.0</v>
+        <v>2013</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>14</v>
@@ -756,9 +830,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <v>43750.55823313657</v>
+        <v>43750.558233136573</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>16</v>
@@ -782,7 +856,7 @@
         <v>13</v>
       </c>
       <c r="I3" s="3">
-        <v>2013.0</v>
+        <v>2013</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>18</v>
@@ -791,7 +865,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>43750.560146759264</v>
       </c>
@@ -817,7 +891,7 @@
         <v>13</v>
       </c>
       <c r="I4" s="3">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>18</v>
@@ -826,9 +900,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
-        <v>43750.56032533565</v>
+        <v>43750.560325335653</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>22</v>
@@ -852,7 +926,7 @@
         <v>23</v>
       </c>
       <c r="I5" s="3">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>24</v>
@@ -861,9 +935,9 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
-        <v>43750.5618527662</v>
+        <v>43750.561852766201</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>26</v>
@@ -896,7 +970,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>43750.57534502315</v>
       </c>
@@ -922,7 +996,7 @@
         <v>13</v>
       </c>
       <c r="I7" s="3">
-        <v>2015.0</v>
+        <v>2015</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>14</v>
@@ -931,9 +1005,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
-        <v>43750.57926278935</v>
+        <v>43750.579262789353</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>31</v>
@@ -957,7 +1031,7 @@
         <v>13</v>
       </c>
       <c r="I8" s="3">
-        <v>2016.0</v>
+        <v>2016</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>18</v>
@@ -966,7 +1040,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>43750.587495162035</v>
       </c>
@@ -1001,9 +1075,9 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
-        <v>43750.58752410879</v>
+        <v>43750.587524108792</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>35</v>
@@ -1027,7 +1101,7 @@
         <v>23</v>
       </c>
       <c r="I10" s="3">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>24</v>
@@ -1036,9 +1110,9 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
-        <v>43750.58915784722</v>
+        <v>43750.589157847222</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>37</v>
@@ -1062,7 +1136,7 @@
         <v>13</v>
       </c>
       <c r="I11" s="3">
-        <v>2015.0</v>
+        <v>2015</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>18</v>
@@ -1071,9 +1145,9 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
-        <v>43750.59281113426</v>
+        <v>43750.592811134258</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>39</v>
@@ -1097,7 +1171,7 @@
         <v>13</v>
       </c>
       <c r="I12" s="3">
-        <v>2015.0</v>
+        <v>2015</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>18</v>
@@ -1106,7 +1180,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>43750.616136655095</v>
       </c>
@@ -1132,7 +1206,7 @@
         <v>13</v>
       </c>
       <c r="I13" s="3">
-        <v>2016.0</v>
+        <v>2016</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>18</v>
@@ -1141,9 +1215,9 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
-        <v>43750.62160413194</v>
+        <v>43750.621604131942</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>43</v>
@@ -1167,7 +1241,7 @@
         <v>23</v>
       </c>
       <c r="I14" s="3">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>14</v>
@@ -1176,7 +1250,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>43750.642080844904</v>
       </c>
@@ -1202,7 +1276,7 @@
         <v>13</v>
       </c>
       <c r="I15" s="3">
-        <v>2011.0</v>
+        <v>2011</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>18</v>
@@ -1211,7 +1285,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>43750.66035150463</v>
       </c>
@@ -1246,7 +1320,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>43750.672098310184</v>
       </c>
@@ -1272,7 +1346,7 @@
         <v>13</v>
       </c>
       <c r="I17" s="3">
-        <v>2015.0</v>
+        <v>2015</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>18</v>
@@ -1281,7 +1355,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>43750.680671678245</v>
       </c>
@@ -1307,7 +1381,7 @@
         <v>13</v>
       </c>
       <c r="I18" s="3">
-        <v>2016.0</v>
+        <v>2016</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>18</v>
@@ -1316,9 +1390,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
-        <v>43750.69628875</v>
+        <v>43750.696288749998</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>53</v>
@@ -1342,7 +1416,7 @@
         <v>13</v>
       </c>
       <c r="I19" s="3">
-        <v>2015.0</v>
+        <v>2015</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>18</v>
@@ -1351,7 +1425,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>43750.762747835644</v>
       </c>
@@ -1386,7 +1460,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>43750.808169930555</v>
       </c>
@@ -1412,7 +1486,7 @@
         <v>13</v>
       </c>
       <c r="I21" s="3">
-        <v>2016.0</v>
+        <v>2016</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>24</v>
@@ -1421,9 +1495,9 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
-        <v>43750.86153310185</v>
+        <v>43750.861533101852</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>60</v>
@@ -1447,7 +1521,7 @@
         <v>23</v>
       </c>
       <c r="I22" s="3">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>14</v>
@@ -1456,7 +1530,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>43750.972747210646</v>
       </c>
@@ -1482,7 +1556,7 @@
         <v>13</v>
       </c>
       <c r="I23" s="3">
-        <v>2016.0</v>
+        <v>2016</v>
       </c>
       <c r="J23" s="3" t="s">
         <v>24</v>
@@ -1491,7 +1565,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>43751.063150925926</v>
       </c>
@@ -1517,7 +1591,7 @@
         <v>23</v>
       </c>
       <c r="I24" s="3">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>24</v>
@@ -1526,7 +1600,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>43751.116056631945</v>
       </c>
@@ -1552,7 +1626,7 @@
         <v>13</v>
       </c>
       <c r="I25" s="3">
-        <v>2016.0</v>
+        <v>2016</v>
       </c>
       <c r="J25" s="3" t="s">
         <v>18</v>
@@ -1561,9 +1635,9 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
-        <v>43751.39220122685</v>
+        <v>43751.392201226852</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>68</v>
@@ -1596,7 +1670,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>43751.51955243056</v>
       </c>
@@ -1631,7 +1705,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>43751.547627465276</v>
       </c>
@@ -1657,7 +1731,7 @@
         <v>13</v>
       </c>
       <c r="I28" s="3">
-        <v>2016.0</v>
+        <v>2016</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>18</v>
@@ -1666,9 +1740,9 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
-        <v>43751.64521293981</v>
+        <v>43751.645212939809</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>74</v>
@@ -1692,7 +1766,7 @@
         <v>13</v>
       </c>
       <c r="I29" s="3">
-        <v>2013.0</v>
+        <v>2013</v>
       </c>
       <c r="J29" s="3" t="s">
         <v>14</v>
@@ -1701,9 +1775,9 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
-        <v>43751.65340284722</v>
+        <v>43751.653402847223</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>76</v>
@@ -1727,7 +1801,7 @@
         <v>13</v>
       </c>
       <c r="I30" s="3">
-        <v>2015.0</v>
+        <v>2015</v>
       </c>
       <c r="J30" s="3" t="s">
         <v>18</v>
@@ -1736,9 +1810,9 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
-        <v>43751.65688504629</v>
+        <v>43751.656885046294</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>78</v>
@@ -1762,7 +1836,7 @@
         <v>13</v>
       </c>
       <c r="I31" s="3">
-        <v>2014.0</v>
+        <v>2014</v>
       </c>
       <c r="J31" s="3" t="s">
         <v>18</v>
@@ -1771,9 +1845,9 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
-        <v>43751.73398899306</v>
+        <v>43751.733988993059</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>80</v>
@@ -1797,7 +1871,7 @@
         <v>23</v>
       </c>
       <c r="I32" s="3">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="J32" s="3" t="s">
         <v>14</v>
@@ -1806,9 +1880,9 @@
         <v>81</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
-        <v>43751.83377224537</v>
+        <v>43751.833772245373</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>82</v>
@@ -1832,7 +1906,7 @@
         <v>56</v>
       </c>
       <c r="I33" s="3">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="J33" s="3" t="s">
         <v>18</v>
@@ -1841,9 +1915,9 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
-        <v>43751.93532800926</v>
+        <v>43751.935328009262</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>84</v>
@@ -1876,9 +1950,9 @@
         <v>85</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
-        <v>43751.95392608797</v>
+        <v>43751.953926087968</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>86</v>
@@ -1902,7 +1976,7 @@
         <v>13</v>
       </c>
       <c r="I35" s="3">
-        <v>2015.0</v>
+        <v>2015</v>
       </c>
       <c r="J35" s="3" t="s">
         <v>14</v>
@@ -1911,7 +1985,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>43752.37214172454</v>
       </c>
@@ -1937,7 +2011,7 @@
         <v>23</v>
       </c>
       <c r="I36" s="3">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="J36" s="3" t="s">
         <v>24</v>
@@ -1946,9 +2020,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
-        <v>43752.39871113426</v>
+        <v>43752.398711134258</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>90</v>
@@ -1972,7 +2046,7 @@
         <v>13</v>
       </c>
       <c r="I37" s="3">
-        <v>2013.0</v>
+        <v>2013</v>
       </c>
       <c r="J37" s="3" t="s">
         <v>18</v>
@@ -1981,7 +2055,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>43752.43202576389</v>
       </c>
@@ -2007,7 +2081,7 @@
         <v>13</v>
       </c>
       <c r="I38" s="3">
-        <v>2016.0</v>
+        <v>2016</v>
       </c>
       <c r="J38" s="3" t="s">
         <v>18</v>
@@ -2016,7 +2090,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>43752.446678356486</v>
       </c>
@@ -2042,7 +2116,7 @@
         <v>13</v>
       </c>
       <c r="I39" s="3">
-        <v>2015.0</v>
+        <v>2015</v>
       </c>
       <c r="J39" s="3" t="s">
         <v>18</v>
@@ -2051,7 +2125,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>43752.50799111111</v>
       </c>
@@ -2086,9 +2160,9 @@
         <v>97</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
-        <v>43752.73004734954</v>
+        <v>43752.730047349542</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>98</v>
@@ -2112,7 +2186,7 @@
         <v>13</v>
       </c>
       <c r="I41" s="3">
-        <v>2016.0</v>
+        <v>2016</v>
       </c>
       <c r="J41" s="3" t="s">
         <v>18</v>
@@ -2121,9 +2195,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
-        <v>43752.76837065972</v>
+        <v>43752.768370659724</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>100</v>
@@ -2156,9 +2230,9 @@
         <v>101</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
-        <v>43752.79942332176</v>
+        <v>43752.799423321761</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>102</v>
@@ -2182,7 +2256,7 @@
         <v>56</v>
       </c>
       <c r="I43" s="3">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="J43" s="3" t="s">
         <v>18</v>
@@ -2191,7 +2265,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="44">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>43752.802107766205</v>
       </c>
@@ -2217,7 +2291,7 @@
         <v>56</v>
       </c>
       <c r="I44" s="3">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="J44" s="3" t="s">
         <v>18</v>
@@ -2226,9 +2300,9 @@
         <v>105</v>
       </c>
     </row>
-    <row r="45">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
-        <v>43752.80566381944</v>
+        <v>43752.805663819439</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>106</v>
@@ -2252,7 +2326,7 @@
         <v>56</v>
       </c>
       <c r="I45" s="3">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="J45" s="3" t="s">
         <v>18</v>
@@ -2261,9 +2335,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="46">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
-        <v>43752.8096325</v>
+        <v>43752.809632500001</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>108</v>
@@ -2287,7 +2361,7 @@
         <v>56</v>
       </c>
       <c r="I46" s="3">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="J46" s="3" t="s">
         <v>18</v>
@@ -2296,9 +2370,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="47">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
-        <v>43752.81676324074</v>
+        <v>43752.816763240742</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>110</v>
@@ -2322,7 +2396,7 @@
         <v>56</v>
       </c>
       <c r="I47" s="3">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="J47" s="3" t="s">
         <v>18</v>
@@ -2331,7 +2405,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>43752.834703472225</v>
       </c>
@@ -2357,7 +2431,7 @@
         <v>56</v>
       </c>
       <c r="I48" s="3">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="J48" s="3" t="s">
         <v>18</v>
@@ -2366,7 +2440,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="49">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>43752.842015312504</v>
       </c>
@@ -2401,9 +2475,9 @@
         <v>115</v>
       </c>
     </row>
-    <row r="50">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
-        <v>43752.84415002315</v>
+        <v>43752.844150023149</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>116</v>
@@ -2427,7 +2501,7 @@
         <v>56</v>
       </c>
       <c r="I50" s="3">
-        <v>2016.0</v>
+        <v>2016</v>
       </c>
       <c r="J50" s="3" t="s">
         <v>18</v>
@@ -2436,7 +2510,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="51">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>43752.852451666666</v>
       </c>
@@ -2462,7 +2536,7 @@
         <v>56</v>
       </c>
       <c r="I51" s="3">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="J51" s="3" t="s">
         <v>18</v>
@@ -2471,9 +2545,9 @@
         <v>119</v>
       </c>
     </row>
-    <row r="52">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
-        <v>43752.86520545139</v>
+        <v>43752.865205451388</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>120</v>
@@ -2497,7 +2571,7 @@
         <v>56</v>
       </c>
       <c r="I52" s="3">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="J52" s="3" t="s">
         <v>18</v>
@@ -2506,7 +2580,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>43752.894955578704</v>
       </c>
@@ -2532,7 +2606,7 @@
         <v>13</v>
       </c>
       <c r="I53" s="3">
-        <v>2016.0</v>
+        <v>2016</v>
       </c>
       <c r="J53" s="3" t="s">
         <v>18</v>
@@ -2541,7 +2615,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>43752.91422280093</v>
       </c>
@@ -2567,7 +2641,7 @@
         <v>56</v>
       </c>
       <c r="I54" s="3">
-        <v>2018.0</v>
+        <v>2018</v>
       </c>
       <c r="J54" s="3" t="s">
         <v>18</v>
@@ -2576,9 +2650,9 @@
         <v>125</v>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
-        <v>43752.93435603009</v>
+        <v>43752.934356030091</v>
       </c>
       <c r="B55" s="3" t="s">
         <v>126</v>
@@ -2602,7 +2676,7 @@
         <v>56</v>
       </c>
       <c r="I55" s="3">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="J55" s="3" t="s">
         <v>18</v>
@@ -2611,9 +2685,9 @@
         <v>127</v>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
-        <v>43752.99704627314</v>
+        <v>43752.997046273143</v>
       </c>
       <c r="B56" s="3" t="s">
         <v>128</v>
@@ -2637,7 +2711,7 @@
         <v>13</v>
       </c>
       <c r="I56" s="3">
-        <v>2013.0</v>
+        <v>2013</v>
       </c>
       <c r="J56" s="3" t="s">
         <v>18</v>
@@ -2646,9 +2720,9 @@
         <v>129</v>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
-        <v>43753.02671481481</v>
+        <v>43753.026714814812</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>130</v>
@@ -2672,7 +2746,7 @@
         <v>56</v>
       </c>
       <c r="I57" s="3">
-        <v>2017.0</v>
+        <v>2017</v>
       </c>
       <c r="J57" s="3" t="s">
         <v>18</v>
@@ -2681,7 +2755,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>43753.360311261575</v>
       </c>
@@ -2707,7 +2781,7 @@
         <v>56</v>
       </c>
       <c r="I58" s="3">
-        <v>2016.0</v>
+        <v>2016</v>
       </c>
       <c r="J58" s="3" t="s">
         <v>18</v>
@@ -2716,9 +2790,9 @@
         <v>133</v>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
-        <v>43753.45336659723</v>
+        <v>43753.453366597227</v>
       </c>
       <c r="B59" s="3" t="s">
         <v>134</v>
@@ -2751,7 +2825,457 @@
         <v>135</v>
       </c>
     </row>
+    <row r="60" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="2">
+        <v>43753.495034722226</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I60" s="3">
+        <v>2019</v>
+      </c>
+      <c r="J60" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K60" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="2">
+        <v>43753.496423611112</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H61" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I61" s="3">
+        <v>2019</v>
+      </c>
+      <c r="J61" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K61" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="2">
+        <v>43753.499895833331</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I62" s="3">
+        <v>2019</v>
+      </c>
+      <c r="J62" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K62" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="2">
+        <v>43754.370034722226</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H63" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I63" s="3">
+        <v>2019</v>
+      </c>
+      <c r="J63" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K63" s="3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="2">
+        <v>43754.432303240741</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I64" s="3">
+        <v>2019</v>
+      </c>
+      <c r="J64" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K64" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="2">
+        <v>43754.439016203702</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I65" s="3">
+        <v>2019</v>
+      </c>
+      <c r="J65" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K65" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="2">
+        <v>43754.494814814818</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I66" s="3">
+        <v>2019</v>
+      </c>
+      <c r="J66" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K66" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="2">
+        <v>43755.411689814813</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H67" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I67" s="3">
+        <v>2019</v>
+      </c>
+      <c r="J67" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K67" s="3" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="2">
+        <v>43755.451527777775</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H68" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I68" s="3">
+        <v>2019</v>
+      </c>
+      <c r="J68" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K68" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="2">
+        <v>43755.466817129629</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E69" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H69" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I69" s="3">
+        <v>2019</v>
+      </c>
+      <c r="J69" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K69" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B70" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C70">
+        <f>COUNTIF(C2:C69,$B$70)</f>
+        <v>64</v>
+      </c>
+      <c r="D70">
+        <f>COUNTIF(D2:D69,$B$70)</f>
+        <v>63</v>
+      </c>
+      <c r="E70">
+        <f>COUNTIF(E2:E69,$B$70)</f>
+        <v>65</v>
+      </c>
+      <c r="F70">
+        <f>COUNTIF(F2:F69,$B$70)</f>
+        <v>10</v>
+      </c>
+      <c r="G70">
+        <f>COUNTIF(G2:G69,$B$70)</f>
+        <v>56</v>
+      </c>
+      <c r="H70">
+        <f>COUNTIF(H2:H69,"Universidad Panamericana")</f>
+        <v>17</v>
+      </c>
+      <c r="J70">
+        <f>COUNTIF(J2:J69,"Si")</f>
+        <v>52</v>
+      </c>
+      <c r="K70" s="3"/>
+    </row>
+    <row r="71" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B71" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C71">
+        <f>COUNTIF(C2:C69,$B$71)</f>
+        <v>2</v>
+      </c>
+      <c r="D71">
+        <f>COUNTIF(D2:D69,$B$71)</f>
+        <v>3</v>
+      </c>
+      <c r="E71">
+        <f>COUNTIF(E2:E69,$B$71)</f>
+        <v>2</v>
+      </c>
+      <c r="F71">
+        <f>COUNTIF(F2:F69,$B$71)</f>
+        <v>20</v>
+      </c>
+      <c r="G71">
+        <f>COUNTIF(G2:G69,$B$71)</f>
+        <v>5</v>
+      </c>
+      <c r="H71">
+        <f>COUNTIF(H2:H69,"ITTG")</f>
+        <v>18</v>
+      </c>
+      <c r="J71">
+        <f>68-J70</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B72" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C72">
+        <f>COUNTIF(C2:C69,$B$72)</f>
+        <v>2</v>
+      </c>
+      <c r="D72">
+        <f>COUNTIF(D2:D69,$B$72)</f>
+        <v>2</v>
+      </c>
+      <c r="E72">
+        <f>COUNTIF(E2:E69,$B$72)</f>
+        <v>1</v>
+      </c>
+      <c r="F72">
+        <f>COUNTIF(F2:F69,$B$72)</f>
+        <v>38</v>
+      </c>
+      <c r="G72">
+        <f>COUNTIF(G2:G69,$B$72)</f>
+        <v>7</v>
+      </c>
+      <c r="H72">
+        <f>COUNTIF(H2:H69,"UPChiapas")</f>
+        <v>33</v>
+      </c>
+      <c r="J72">
+        <f>COUNTIF(J2:J69,$B$72)</f>
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Last course 2019 is included
Last course of year 2019 is included in the survey
</commit_message>
<xml_diff>
--- a/responses/Simulador_SO_Responses.xlsx
+++ b/responses/Simulador_SO_Responses.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clopezp\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clopezp\Documents\GitHub\webOSSimulatorLatex\responses\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -748,11 +748,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K72"/>
+  <dimension ref="A1:K74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H74" sqref="H74:H76"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H71" sqref="H71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -760,7 +760,7 @@
     <col min="1" max="17" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -795,7 +795,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>43750.557912569449</v>
       </c>
@@ -830,7 +830,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>43750.558233136573</v>
       </c>
@@ -865,7 +865,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>43750.560146759264</v>
       </c>
@@ -900,7 +900,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>43750.560325335653</v>
       </c>
@@ -935,7 +935,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>43750.561852766201</v>
       </c>
@@ -970,7 +970,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>43750.57534502315</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>43750.579262789353</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>43750.587495162035</v>
       </c>
@@ -1075,7 +1075,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>43750.587524108792</v>
       </c>
@@ -1110,7 +1110,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>43750.589157847222</v>
       </c>
@@ -1145,7 +1145,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>43750.592811134258</v>
       </c>
@@ -1180,7 +1180,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>43750.616136655095</v>
       </c>
@@ -1215,7 +1215,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>43750.621604131942</v>
       </c>
@@ -1250,7 +1250,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>43750.642080844904</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>43750.66035150463</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>43750.672098310184</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>43750.680671678245</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>43750.696288749998</v>
       </c>
@@ -1425,7 +1425,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>43750.762747835644</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>43750.808169930555</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>43750.861533101852</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>43750.972747210646</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>43751.063150925926</v>
       </c>
@@ -1600,7 +1600,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>43751.116056631945</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>43751.392201226852</v>
       </c>
@@ -1670,7 +1670,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>43751.51955243056</v>
       </c>
@@ -1705,7 +1705,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>43751.547627465276</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>43751.645212939809</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>43751.653402847223</v>
       </c>
@@ -1810,7 +1810,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>43751.656885046294</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>43751.733988993059</v>
       </c>
@@ -1880,7 +1880,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="2">
         <v>43751.833772245373</v>
       </c>
@@ -1915,7 +1915,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>43751.935328009262</v>
       </c>
@@ -1950,7 +1950,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="2">
         <v>43751.953926087968</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>43752.37214172454</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>43752.398711134258</v>
       </c>
@@ -2055,7 +2055,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="2">
         <v>43752.43202576389</v>
       </c>
@@ -2090,7 +2090,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="2">
         <v>43752.446678356486</v>
       </c>
@@ -2125,7 +2125,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>43752.50799111111</v>
       </c>
@@ -2160,7 +2160,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>43752.730047349542</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="2">
         <v>43752.768370659724</v>
       </c>
@@ -2230,7 +2230,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>43752.799423321761</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="2">
         <v>43752.802107766205</v>
       </c>
@@ -2300,7 +2300,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="2">
         <v>43752.805663819439</v>
       </c>
@@ -2335,7 +2335,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
         <v>43752.809632500001</v>
       </c>
@@ -2370,7 +2370,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>43752.816763240742</v>
       </c>
@@ -2405,7 +2405,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="2">
         <v>43752.834703472225</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="2">
         <v>43752.842015312504</v>
       </c>
@@ -2475,7 +2475,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="2">
         <v>43752.844150023149</v>
       </c>
@@ -2510,7 +2510,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="2">
         <v>43752.852451666666</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="2">
         <v>43752.865205451388</v>
       </c>
@@ -2580,7 +2580,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="2">
         <v>43752.894955578704</v>
       </c>
@@ -2615,7 +2615,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="2">
         <v>43752.91422280093</v>
       </c>
@@ -2650,7 +2650,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="2">
         <v>43752.934356030091</v>
       </c>
@@ -2685,7 +2685,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="2">
         <v>43752.997046273143</v>
       </c>
@@ -2720,7 +2720,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="2">
         <v>43753.026714814812</v>
       </c>
@@ -2755,7 +2755,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="2">
         <v>43753.360311261575</v>
       </c>
@@ -2790,7 +2790,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="2">
         <v>43753.453366597227</v>
       </c>
@@ -2854,7 +2854,7 @@
         <v>2019</v>
       </c>
       <c r="J60" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="K60" s="3" t="s">
         <v>145</v>
@@ -2889,7 +2889,7 @@
         <v>2019</v>
       </c>
       <c r="J61" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="K61" s="3" t="s">
         <v>146</v>
@@ -2924,7 +2924,7 @@
         <v>2019</v>
       </c>
       <c r="J62" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="K62" s="3" t="s">
         <v>147</v>
@@ -2959,7 +2959,7 @@
         <v>2019</v>
       </c>
       <c r="J63" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="K63" s="3" t="s">
         <v>148</v>
@@ -2994,7 +2994,7 @@
         <v>2019</v>
       </c>
       <c r="J64" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="K64" s="3" t="s">
         <v>149</v>
@@ -3029,7 +3029,7 @@
         <v>2019</v>
       </c>
       <c r="J65" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="K65" s="3" t="s">
         <v>150</v>
@@ -3064,7 +3064,7 @@
         <v>2019</v>
       </c>
       <c r="J66" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="K66" s="3" t="s">
         <v>151</v>
@@ -3099,7 +3099,7 @@
         <v>2019</v>
       </c>
       <c r="J67" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="K67" s="3" t="s">
         <v>152</v>
@@ -3205,7 +3205,7 @@
       </c>
       <c r="J70">
         <f>COUNTIF(J2:J69,"Si")</f>
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="K70" s="3"/>
     </row>
@@ -3239,7 +3239,7 @@
       </c>
       <c r="J71">
         <f>68-J70</f>
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="72" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3273,6 +3273,18 @@
       <c r="J72">
         <f>COUNTIF(J2:J69,$B$72)</f>
         <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J73">
+        <f>SUM(J70:J72)</f>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J74">
+        <f>(44*100)/68</f>
+        <v>64.705882352941174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>